<commit_message>
updated 1988 Georgia, Hawaii & added 1988 Idaho, Illinois
</commit_message>
<xml_diff>
--- a/Output/1988/Georgia/Georgia.xlsx
+++ b/Output/1988/Georgia/Georgia.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$AA$530</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$Z$530</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4013" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="720">
   <si>
     <t>Name</t>
   </si>
@@ -2166,9 +2166,6 @@
   </si>
   <si>
     <t>Includes subscribers, miles of plant &amp; homes passed figures for Cuthbert, Fulton County, Rockmore &amp; Villa Rica, GA.</t>
-  </si>
-  <si>
-    <t>Alert</t>
   </si>
   <si>
     <t>See HOMERVILLE, GA</t>
@@ -2561,7 +2558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7D810D-891D-1E49-9D1A-99F2A206D9FE}">
-  <dimension ref="A1:AA530"/>
+  <dimension ref="A1:Z530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2570,9 +2567,9 @@
     <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2649,13 +2646,10 @@
       <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -2727,9 +2721,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -2801,9 +2795,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -2875,9 +2869,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -2949,9 +2943,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -3026,9 +3020,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
@@ -3100,9 +3094,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
@@ -3174,12 +3168,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B9" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -3248,9 +3242,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -3322,9 +3316,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -3396,9 +3390,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
@@ -3470,9 +3464,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
@@ -3544,9 +3538,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B14" t="s">
         <v>67</v>
@@ -3618,9 +3612,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B15" t="s">
         <v>70</v>
@@ -3692,12 +3686,12 @@
         <v>71</v>
       </c>
       <c r="Z15" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B16" t="s">
         <v>74</v>
@@ -3771,7 +3765,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B17" t="s">
         <v>85</v>
@@ -3845,7 +3839,7 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B18" t="s">
         <v>97</v>
@@ -3919,7 +3913,7 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B19" t="s">
         <v>98</v>
@@ -3993,7 +3987,7 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B20" t="s">
         <v>101</v>
@@ -4067,7 +4061,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B21" t="s">
         <v>104</v>
@@ -4141,7 +4135,7 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B22" t="s">
         <v>107</v>
@@ -4215,7 +4209,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B23" t="s">
         <v>112</v>
@@ -4289,7 +4283,7 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B24" t="s">
         <v>125</v>
@@ -4363,7 +4357,7 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B25" t="s">
         <v>130</v>
@@ -4437,7 +4431,7 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B26" t="s">
         <v>137</v>
@@ -4511,7 +4505,7 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B27" t="s">
         <v>138</v>
@@ -4585,7 +4579,7 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B28" t="s">
         <v>144</v>
@@ -4659,7 +4653,7 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B29" t="s">
         <v>149</v>
@@ -4733,7 +4727,7 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B30" t="s">
         <v>152</v>
@@ -4807,7 +4801,7 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B31" t="s">
         <v>155</v>
@@ -4881,7 +4875,7 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B32" t="s">
         <v>157</v>
@@ -4955,7 +4949,7 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B33" t="s">
         <v>164</v>
@@ -4970,7 +4964,7 @@
         <v>28611</v>
       </c>
       <c r="G33" s="2">
-        <v>4226</v>
+        <v>600</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
@@ -5029,7 +5023,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B34" t="s">
         <v>167</v>
@@ -5103,7 +5097,7 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B35" t="s">
         <v>168</v>
@@ -5177,7 +5171,7 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B36" t="s">
         <v>170</v>
@@ -5251,7 +5245,7 @@
     </row>
     <row r="37" spans="1:25">
       <c r="A37" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B37" t="s">
         <v>173</v>
@@ -5325,7 +5319,7 @@
     </row>
     <row r="38" spans="1:25">
       <c r="A38" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B38" t="s">
         <v>176</v>
@@ -5399,7 +5393,7 @@
     </row>
     <row r="39" spans="1:25">
       <c r="A39" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B39" t="s">
         <v>184</v>
@@ -5473,7 +5467,7 @@
     </row>
     <row r="40" spans="1:25">
       <c r="A40" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B40" t="s">
         <v>193</v>
@@ -5547,7 +5541,7 @@
     </row>
     <row r="41" spans="1:25">
       <c r="A41" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B41" t="s">
         <v>194</v>
@@ -5621,7 +5615,7 @@
     </row>
     <row r="42" spans="1:25">
       <c r="A42" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B42" t="s">
         <v>195</v>
@@ -5695,7 +5689,7 @@
     </row>
     <row r="43" spans="1:25">
       <c r="A43" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B43" t="s">
         <v>200</v>
@@ -5769,7 +5763,7 @@
     </row>
     <row r="44" spans="1:25">
       <c r="A44" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B44" t="s">
         <v>203</v>
@@ -5843,7 +5837,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B45" t="s">
         <v>217</v>
@@ -5917,7 +5911,7 @@
     </row>
     <row r="46" spans="1:25">
       <c r="A46" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B46" t="s">
         <v>217</v>
@@ -5991,7 +5985,7 @@
     </row>
     <row r="47" spans="1:25">
       <c r="A47" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B47" t="s">
         <v>219</v>
@@ -6065,7 +6059,7 @@
     </row>
     <row r="48" spans="1:25">
       <c r="A48" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B48" t="s">
         <v>220</v>
@@ -6139,7 +6133,7 @@
     </row>
     <row r="49" spans="1:25">
       <c r="A49" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B49" t="s">
         <v>221</v>
@@ -6213,7 +6207,7 @@
     </row>
     <row r="50" spans="1:25">
       <c r="A50" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B50" t="s">
         <v>222</v>
@@ -6287,7 +6281,7 @@
     </row>
     <row r="51" spans="1:25">
       <c r="A51" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B51" t="s">
         <v>223</v>
@@ -6361,7 +6355,7 @@
     </row>
     <row r="52" spans="1:25">
       <c r="A52" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B52" t="s">
         <v>228</v>
@@ -6435,7 +6429,7 @@
     </row>
     <row r="53" spans="1:25">
       <c r="A53" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B53" t="s">
         <v>229</v>
@@ -6509,7 +6503,7 @@
     </row>
     <row r="54" spans="1:25">
       <c r="A54" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B54" t="s">
         <v>230</v>
@@ -6583,7 +6577,7 @@
     </row>
     <row r="55" spans="1:25">
       <c r="A55" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B55" t="s">
         <v>235</v>
@@ -6657,7 +6651,7 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B56" t="s">
         <v>236</v>
@@ -6731,7 +6725,7 @@
     </row>
     <row r="57" spans="1:25">
       <c r="A57" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B57" t="s">
         <v>237</v>
@@ -6805,7 +6799,7 @@
     </row>
     <row r="58" spans="1:25">
       <c r="A58" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B58" t="s">
         <v>241</v>
@@ -6879,7 +6873,7 @@
     </row>
     <row r="59" spans="1:25">
       <c r="A59" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B59" t="s">
         <v>243</v>
@@ -6953,7 +6947,7 @@
     </row>
     <row r="60" spans="1:25">
       <c r="A60" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B60" t="s">
         <v>254</v>
@@ -7027,7 +7021,7 @@
     </row>
     <row r="61" spans="1:25">
       <c r="A61" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B61" t="s">
         <v>257</v>
@@ -7101,7 +7095,7 @@
     </row>
     <row r="62" spans="1:25">
       <c r="A62" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B62" t="s">
         <v>259</v>
@@ -7175,7 +7169,7 @@
     </row>
     <row r="63" spans="1:25">
       <c r="A63" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B63" t="s">
         <v>260</v>
@@ -7249,7 +7243,7 @@
     </row>
     <row r="64" spans="1:25">
       <c r="A64" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B64" t="s">
         <v>265</v>
@@ -7323,7 +7317,7 @@
     </row>
     <row r="65" spans="1:26">
       <c r="A65" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B65" t="s">
         <v>266</v>
@@ -7397,7 +7391,7 @@
     </row>
     <row r="66" spans="1:26">
       <c r="A66" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B66" t="s">
         <v>274</v>
@@ -7471,7 +7465,7 @@
     </row>
     <row r="67" spans="1:26">
       <c r="A67" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B67" t="s">
         <v>277</v>
@@ -7545,7 +7539,7 @@
     </row>
     <row r="68" spans="1:26">
       <c r="A68" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B68" t="s">
         <v>280</v>
@@ -7619,7 +7613,7 @@
     </row>
     <row r="69" spans="1:26">
       <c r="A69" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B69" t="s">
         <v>285</v>
@@ -7693,7 +7687,7 @@
     </row>
     <row r="70" spans="1:26">
       <c r="A70" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B70" t="s">
         <v>288</v>
@@ -7767,7 +7761,7 @@
     </row>
     <row r="71" spans="1:26">
       <c r="A71" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B71" t="s">
         <v>292</v>
@@ -7841,7 +7835,7 @@
     </row>
     <row r="72" spans="1:26">
       <c r="A72" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B72" t="s">
         <v>302</v>
@@ -7915,7 +7909,7 @@
     </row>
     <row r="73" spans="1:26">
       <c r="A73" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B73" t="s">
         <v>305</v>
@@ -7989,7 +7983,7 @@
     </row>
     <row r="74" spans="1:26">
       <c r="A74" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B74" t="s">
         <v>306</v>
@@ -8061,12 +8055,12 @@
         <v>307</v>
       </c>
       <c r="Z74" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="75" spans="1:26">
       <c r="A75" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B75" t="s">
         <v>308</v>
@@ -8140,7 +8134,7 @@
     </row>
     <row r="76" spans="1:26">
       <c r="A76" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B76" t="s">
         <v>311</v>
@@ -8214,7 +8208,7 @@
     </row>
     <row r="77" spans="1:26">
       <c r="A77" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B77" t="s">
         <v>315</v>
@@ -8288,7 +8282,7 @@
     </row>
     <row r="78" spans="1:26">
       <c r="A78" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B78" t="s">
         <v>318</v>
@@ -8362,7 +8356,7 @@
     </row>
     <row r="79" spans="1:26">
       <c r="A79" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B79" t="s">
         <v>321</v>
@@ -8436,7 +8430,7 @@
     </row>
     <row r="80" spans="1:26">
       <c r="A80" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B80" t="s">
         <v>329</v>
@@ -8510,7 +8504,7 @@
     </row>
     <row r="81" spans="1:25">
       <c r="A81" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B81" t="s">
         <v>334</v>
@@ -8584,7 +8578,7 @@
     </row>
     <row r="82" spans="1:25">
       <c r="A82" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B82" t="s">
         <v>338</v>
@@ -8658,7 +8652,7 @@
     </row>
     <row r="83" spans="1:25">
       <c r="A83" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B83" t="s">
         <v>344</v>
@@ -8732,7 +8726,7 @@
     </row>
     <row r="84" spans="1:25">
       <c r="A84" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B84" t="s">
         <v>345</v>
@@ -8806,7 +8800,7 @@
     </row>
     <row r="85" spans="1:25">
       <c r="A85" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B85" t="s">
         <v>346</v>
@@ -8880,7 +8874,7 @@
     </row>
     <row r="86" spans="1:25">
       <c r="A86" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B86" t="s">
         <v>347</v>
@@ -8954,7 +8948,7 @@
     </row>
     <row r="87" spans="1:25">
       <c r="A87" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B87" t="s">
         <v>348</v>
@@ -9028,7 +9022,7 @@
     </row>
     <row r="88" spans="1:25">
       <c r="A88" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B88" t="s">
         <v>350</v>
@@ -9102,7 +9096,7 @@
     </row>
     <row r="89" spans="1:25">
       <c r="A89" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B89" t="s">
         <v>352</v>
@@ -9176,7 +9170,7 @@
     </row>
     <row r="90" spans="1:25">
       <c r="A90" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B90" t="s">
         <v>367</v>
@@ -9250,7 +9244,7 @@
     </row>
     <row r="91" spans="1:25">
       <c r="A91" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B91" t="s">
         <v>368</v>
@@ -9324,7 +9318,7 @@
     </row>
     <row r="92" spans="1:25">
       <c r="A92" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B92" t="s">
         <v>369</v>
@@ -9398,7 +9392,7 @@
     </row>
     <row r="93" spans="1:25">
       <c r="A93" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B93" t="s">
         <v>370</v>
@@ -9472,7 +9466,7 @@
     </row>
     <row r="94" spans="1:25">
       <c r="A94" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B94" t="s">
         <v>376</v>
@@ -9546,7 +9540,7 @@
     </row>
     <row r="95" spans="1:25">
       <c r="A95" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B95" t="s">
         <v>379</v>
@@ -9620,7 +9614,7 @@
     </row>
     <row r="96" spans="1:25">
       <c r="A96" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B96" t="s">
         <v>385</v>
@@ -9694,7 +9688,7 @@
     </row>
     <row r="97" spans="1:25">
       <c r="A97" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B97" t="s">
         <v>393</v>
@@ -9768,7 +9762,7 @@
     </row>
     <row r="98" spans="1:25">
       <c r="A98" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B98" t="s">
         <v>397</v>
@@ -9842,7 +9836,7 @@
     </row>
     <row r="99" spans="1:25">
       <c r="A99" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B99" t="s">
         <v>400</v>
@@ -9916,7 +9910,7 @@
     </row>
     <row r="100" spans="1:25">
       <c r="A100" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B100" t="s">
         <v>404</v>
@@ -9990,7 +9984,7 @@
     </row>
     <row r="101" spans="1:25">
       <c r="A101" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B101" t="s">
         <v>409</v>
@@ -10064,7 +10058,7 @@
     </row>
     <row r="102" spans="1:25">
       <c r="A102" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B102" t="s">
         <v>411</v>
@@ -10138,7 +10132,7 @@
     </row>
     <row r="103" spans="1:25">
       <c r="A103" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B103" t="s">
         <v>413</v>
@@ -10212,7 +10206,7 @@
     </row>
     <row r="104" spans="1:25">
       <c r="A104" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B104" t="s">
         <v>414</v>
@@ -10286,7 +10280,7 @@
     </row>
     <row r="105" spans="1:25">
       <c r="A105" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B105" t="s">
         <v>418</v>
@@ -10360,7 +10354,7 @@
     </row>
     <row r="106" spans="1:25">
       <c r="A106" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B106" t="s">
         <v>419</v>
@@ -10434,7 +10428,7 @@
     </row>
     <row r="107" spans="1:25">
       <c r="A107" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B107" t="s">
         <v>426</v>
@@ -10508,7 +10502,7 @@
     </row>
     <row r="108" spans="1:25">
       <c r="A108" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B108" t="s">
         <v>427</v>
@@ -10582,7 +10576,7 @@
     </row>
     <row r="109" spans="1:25">
       <c r="A109" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B109" t="s">
         <v>432</v>
@@ -10656,7 +10650,7 @@
     </row>
     <row r="110" spans="1:25">
       <c r="A110" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B110" t="s">
         <v>441</v>
@@ -10730,7 +10724,7 @@
     </row>
     <row r="111" spans="1:25">
       <c r="A111" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B111" t="s">
         <v>443</v>
@@ -10804,7 +10798,7 @@
     </row>
     <row r="112" spans="1:25">
       <c r="A112" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B112" t="s">
         <v>446</v>
@@ -10878,7 +10872,7 @@
     </row>
     <row r="113" spans="1:25">
       <c r="A113" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B113" t="s">
         <v>453</v>
@@ -10952,7 +10946,7 @@
     </row>
     <row r="114" spans="1:25">
       <c r="A114" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B114" t="s">
         <v>457</v>
@@ -11026,7 +11020,7 @@
     </row>
     <row r="115" spans="1:25">
       <c r="A115" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B115" t="s">
         <v>459</v>
@@ -11100,7 +11094,7 @@
     </row>
     <row r="116" spans="1:25">
       <c r="A116" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B116" t="s">
         <v>460</v>
@@ -11174,7 +11168,7 @@
     </row>
     <row r="117" spans="1:25">
       <c r="A117" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B117" t="s">
         <v>467</v>
@@ -11248,7 +11242,7 @@
     </row>
     <row r="118" spans="1:25">
       <c r="A118" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B118" t="s">
         <v>472</v>
@@ -11322,7 +11316,7 @@
     </row>
     <row r="119" spans="1:25">
       <c r="A119" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B119" t="s">
         <v>475</v>
@@ -11396,7 +11390,7 @@
     </row>
     <row r="120" spans="1:25">
       <c r="A120" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B120" t="s">
         <v>476</v>
@@ -11470,7 +11464,7 @@
     </row>
     <row r="121" spans="1:25">
       <c r="A121" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B121" t="s">
         <v>477</v>
@@ -11544,7 +11538,7 @@
     </row>
     <row r="122" spans="1:25">
       <c r="A122" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B122" t="s">
         <v>478</v>
@@ -11618,7 +11612,7 @@
     </row>
     <row r="123" spans="1:25">
       <c r="A123" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B123" t="s">
         <v>479</v>
@@ -11692,7 +11686,7 @@
     </row>
     <row r="124" spans="1:25">
       <c r="A124" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B124" t="s">
         <v>480</v>
@@ -11766,7 +11760,7 @@
     </row>
     <row r="125" spans="1:25">
       <c r="A125" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B125" t="s">
         <v>483</v>
@@ -11840,7 +11834,7 @@
     </row>
     <row r="126" spans="1:25">
       <c r="A126" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B126" t="s">
         <v>484</v>
@@ -11914,7 +11908,7 @@
     </row>
     <row r="127" spans="1:25">
       <c r="A127" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B127" t="s">
         <v>487</v>
@@ -11988,7 +11982,7 @@
     </row>
     <row r="128" spans="1:25">
       <c r="A128" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B128" t="s">
         <v>488</v>
@@ -12062,7 +12056,7 @@
     </row>
     <row r="129" spans="1:26">
       <c r="A129" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B129" t="s">
         <v>494</v>
@@ -12136,7 +12130,7 @@
     </row>
     <row r="130" spans="1:26">
       <c r="A130" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B130" t="s">
         <v>496</v>
@@ -12210,7 +12204,7 @@
     </row>
     <row r="131" spans="1:26">
       <c r="A131" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B131" t="s">
         <v>501</v>
@@ -12284,7 +12278,7 @@
     </row>
     <row r="132" spans="1:26">
       <c r="A132" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B132" t="s">
         <v>502</v>
@@ -12358,7 +12352,7 @@
     </row>
     <row r="133" spans="1:26">
       <c r="A133" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B133" t="s">
         <v>503</v>
@@ -12432,7 +12426,7 @@
     </row>
     <row r="134" spans="1:26">
       <c r="A134" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B134" t="s">
         <v>513</v>
@@ -12506,7 +12500,7 @@
     </row>
     <row r="135" spans="1:26">
       <c r="A135" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B135" t="s">
         <v>518</v>
@@ -12580,7 +12574,7 @@
     </row>
     <row r="136" spans="1:26">
       <c r="A136" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B136" t="s">
         <v>521</v>
@@ -12657,7 +12651,7 @@
     </row>
     <row r="137" spans="1:26">
       <c r="A137" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B137" t="s">
         <v>522</v>
@@ -12731,7 +12725,7 @@
     </row>
     <row r="138" spans="1:26">
       <c r="A138" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B138" t="s">
         <v>524</v>
@@ -12805,7 +12799,7 @@
     </row>
     <row r="139" spans="1:26">
       <c r="A139" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B139" t="s">
         <v>526</v>
@@ -12879,7 +12873,7 @@
     </row>
     <row r="140" spans="1:26">
       <c r="A140" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B140" t="s">
         <v>531</v>
@@ -12953,7 +12947,7 @@
     </row>
     <row r="141" spans="1:26">
       <c r="A141" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B141" t="s">
         <v>533</v>
@@ -13027,7 +13021,7 @@
     </row>
     <row r="142" spans="1:26">
       <c r="A142" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B142" t="s">
         <v>536</v>
@@ -13101,7 +13095,7 @@
     </row>
     <row r="143" spans="1:26">
       <c r="A143" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B143" t="s">
         <v>544</v>
@@ -13175,7 +13169,7 @@
     </row>
     <row r="144" spans="1:26">
       <c r="A144" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B144" t="s">
         <v>550</v>
@@ -13249,7 +13243,7 @@
     </row>
     <row r="145" spans="1:25">
       <c r="A145" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B145" t="s">
         <v>556</v>
@@ -13323,7 +13317,7 @@
     </row>
     <row r="146" spans="1:25">
       <c r="A146" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B146" t="s">
         <v>560</v>
@@ -13397,7 +13391,7 @@
     </row>
     <row r="147" spans="1:25">
       <c r="A147" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B147" t="s">
         <v>564</v>
@@ -13471,7 +13465,7 @@
     </row>
     <row r="148" spans="1:25">
       <c r="A148" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B148" t="s">
         <v>565</v>
@@ -13545,7 +13539,7 @@
     </row>
     <row r="149" spans="1:25">
       <c r="A149" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B149" t="s">
         <v>567</v>
@@ -13619,7 +13613,7 @@
     </row>
     <row r="150" spans="1:25">
       <c r="A150" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B150" t="s">
         <v>568</v>
@@ -13693,7 +13687,7 @@
     </row>
     <row r="151" spans="1:25">
       <c r="A151" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B151" t="s">
         <v>569</v>
@@ -13767,7 +13761,7 @@
     </row>
     <row r="152" spans="1:25">
       <c r="A152" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B152" t="s">
         <v>572</v>
@@ -13841,7 +13835,7 @@
     </row>
     <row r="153" spans="1:25">
       <c r="A153" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B153" t="s">
         <v>574</v>
@@ -13915,7 +13909,7 @@
     </row>
     <row r="154" spans="1:25">
       <c r="A154" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B154" t="s">
         <v>575</v>
@@ -13989,7 +13983,7 @@
     </row>
     <row r="155" spans="1:25">
       <c r="A155" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B155" t="s">
         <v>575</v>
@@ -14063,7 +14057,7 @@
     </row>
     <row r="156" spans="1:25">
       <c r="A156" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B156" t="s">
         <v>576</v>
@@ -14137,7 +14131,7 @@
     </row>
     <row r="157" spans="1:25">
       <c r="A157" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B157" t="s">
         <v>577</v>
@@ -14211,7 +14205,7 @@
     </row>
     <row r="158" spans="1:25">
       <c r="A158" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B158" t="s">
         <v>579</v>
@@ -14285,7 +14279,7 @@
     </row>
     <row r="159" spans="1:25">
       <c r="A159" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B159" t="s">
         <v>581</v>
@@ -14359,7 +14353,7 @@
     </row>
     <row r="160" spans="1:25">
       <c r="A160" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B160" t="s">
         <v>585</v>
@@ -14433,7 +14427,7 @@
     </row>
     <row r="161" spans="1:25">
       <c r="A161" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B161" t="s">
         <v>586</v>
@@ -14507,7 +14501,7 @@
     </row>
     <row r="162" spans="1:25">
       <c r="A162" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B162" t="s">
         <v>592</v>
@@ -14581,7 +14575,7 @@
     </row>
     <row r="163" spans="1:25">
       <c r="A163" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B163" t="s">
         <v>593</v>
@@ -14655,7 +14649,7 @@
     </row>
     <row r="164" spans="1:25">
       <c r="A164" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B164" t="s">
         <v>594</v>
@@ -14729,7 +14723,7 @@
     </row>
     <row r="165" spans="1:25">
       <c r="A165" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B165" t="s">
         <v>600</v>
@@ -14803,7 +14797,7 @@
     </row>
     <row r="166" spans="1:25">
       <c r="A166" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B166" t="s">
         <v>606</v>
@@ -14877,7 +14871,7 @@
     </row>
     <row r="167" spans="1:25">
       <c r="A167" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B167" t="s">
         <v>607</v>
@@ -14951,7 +14945,7 @@
     </row>
     <row r="168" spans="1:25">
       <c r="A168" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B168" t="s">
         <v>608</v>
@@ -15025,7 +15019,7 @@
     </row>
     <row r="169" spans="1:25">
       <c r="A169" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B169" t="s">
         <v>614</v>
@@ -15099,7 +15093,7 @@
     </row>
     <row r="170" spans="1:25">
       <c r="A170" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B170" t="s">
         <v>617</v>
@@ -15173,7 +15167,7 @@
     </row>
     <row r="171" spans="1:25">
       <c r="A171" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B171" t="s">
         <v>618</v>
@@ -15247,7 +15241,7 @@
     </row>
     <row r="172" spans="1:25">
       <c r="A172" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B172" t="s">
         <v>619</v>
@@ -15321,7 +15315,7 @@
     </row>
     <row r="173" spans="1:25">
       <c r="A173" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B173" t="s">
         <v>620</v>
@@ -15395,7 +15389,7 @@
     </row>
     <row r="174" spans="1:25">
       <c r="A174" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B174" t="s">
         <v>621</v>
@@ -15469,7 +15463,7 @@
     </row>
     <row r="175" spans="1:25">
       <c r="A175" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B175" t="s">
         <v>625</v>
@@ -15543,7 +15537,7 @@
     </row>
     <row r="176" spans="1:25">
       <c r="A176" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B176" t="s">
         <v>626</v>
@@ -15617,7 +15611,7 @@
     </row>
     <row r="177" spans="1:25">
       <c r="A177" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B177" t="s">
         <v>627</v>
@@ -15691,7 +15685,7 @@
     </row>
     <row r="178" spans="1:25">
       <c r="A178" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B178" t="s">
         <v>629</v>
@@ -15765,7 +15759,7 @@
     </row>
     <row r="179" spans="1:25">
       <c r="A179" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B179" t="s">
         <v>630</v>
@@ -15839,7 +15833,7 @@
     </row>
     <row r="180" spans="1:25">
       <c r="A180" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B180" t="s">
         <v>631</v>
@@ -15913,7 +15907,7 @@
     </row>
     <row r="181" spans="1:25">
       <c r="A181" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B181" t="s">
         <v>636</v>
@@ -15987,7 +15981,7 @@
     </row>
     <row r="182" spans="1:25">
       <c r="A182" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B182" t="s">
         <v>643</v>
@@ -16061,7 +16055,7 @@
     </row>
     <row r="183" spans="1:25">
       <c r="A183" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B183" t="s">
         <v>644</v>
@@ -16135,7 +16129,7 @@
     </row>
     <row r="184" spans="1:25">
       <c r="A184" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B184" t="s">
         <v>648</v>
@@ -16209,7 +16203,7 @@
     </row>
     <row r="185" spans="1:25">
       <c r="A185" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B185" t="s">
         <v>651</v>
@@ -16283,7 +16277,7 @@
     </row>
     <row r="186" spans="1:25">
       <c r="A186" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B186" t="s">
         <v>657</v>
@@ -16357,7 +16351,7 @@
     </row>
     <row r="187" spans="1:25">
       <c r="A187" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B187" t="s">
         <v>706</v>
@@ -16431,7 +16425,7 @@
     </row>
     <row r="188" spans="1:25">
       <c r="A188" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B188" t="s">
         <v>664</v>
@@ -16505,7 +16499,7 @@
     </row>
     <row r="189" spans="1:25">
       <c r="A189" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B189" t="s">
         <v>671</v>
@@ -16579,7 +16573,7 @@
     </row>
     <row r="190" spans="1:25">
       <c r="A190" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B190" t="s">
         <v>674</v>
@@ -16653,7 +16647,7 @@
     </row>
     <row r="191" spans="1:25">
       <c r="A191" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B191" t="s">
         <v>676</v>
@@ -16727,7 +16721,7 @@
     </row>
     <row r="192" spans="1:25">
       <c r="A192" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B192" t="s">
         <v>677</v>
@@ -16801,7 +16795,7 @@
     </row>
     <row r="193" spans="1:25">
       <c r="A193" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B193" t="s">
         <v>678</v>
@@ -16875,7 +16869,7 @@
     </row>
     <row r="194" spans="1:25">
       <c r="A194" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B194" t="s">
         <v>679</v>
@@ -16949,7 +16943,7 @@
     </row>
     <row r="195" spans="1:25">
       <c r="A195" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B195" t="s">
         <v>688</v>
@@ -17023,7 +17017,7 @@
     </row>
     <row r="196" spans="1:25">
       <c r="A196" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B196" t="s">
         <v>690</v>
@@ -17097,7 +17091,7 @@
     </row>
     <row r="197" spans="1:25">
       <c r="A197" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B197" t="s">
         <v>691</v>
@@ -17171,7 +17165,7 @@
     </row>
     <row r="198" spans="1:25">
       <c r="A198" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B198" t="s">
         <v>692</v>
@@ -17245,7 +17239,7 @@
     </row>
     <row r="199" spans="1:25">
       <c r="A199" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B199" t="s">
         <v>694</v>
@@ -17319,7 +17313,7 @@
     </row>
     <row r="200" spans="1:25">
       <c r="A200" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B200" t="s">
         <v>695</v>
@@ -17393,7 +17387,7 @@
     </row>
     <row r="201" spans="1:25">
       <c r="A201" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B201" t="s">
         <v>697</v>
@@ -17467,7 +17461,7 @@
     </row>
     <row r="202" spans="1:25">
       <c r="A202" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B202" t="s">
         <v>29</v>
@@ -17481,7 +17475,7 @@
     </row>
     <row r="203" spans="1:25">
       <c r="A203" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B203" t="s">
         <v>33</v>
@@ -17495,7 +17489,7 @@
     </row>
     <row r="204" spans="1:25">
       <c r="A204" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B204" t="s">
         <v>36</v>
@@ -17509,7 +17503,7 @@
     </row>
     <row r="205" spans="1:25">
       <c r="A205" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B205" t="s">
         <v>38</v>
@@ -17523,7 +17517,7 @@
     </row>
     <row r="206" spans="1:25">
       <c r="A206" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B206" t="s">
         <v>45</v>
@@ -17537,7 +17531,7 @@
     </row>
     <row r="207" spans="1:25">
       <c r="A207" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B207" t="s">
         <v>47</v>
@@ -17551,7 +17545,7 @@
     </row>
     <row r="208" spans="1:25">
       <c r="A208" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B208" t="s">
         <v>51</v>
@@ -17565,7 +17559,7 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B209" t="s">
         <v>53</v>
@@ -17579,7 +17573,7 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B210" t="s">
         <v>57</v>
@@ -17593,7 +17587,7 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B211" t="s">
         <v>59</v>
@@ -17607,7 +17601,7 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B212" t="s">
         <v>65</v>
@@ -17621,7 +17615,7 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B213" t="s">
         <v>66</v>
@@ -17635,7 +17629,7 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B214" t="s">
         <v>69</v>
@@ -17649,7 +17643,7 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B215" t="s">
         <v>72</v>
@@ -17663,7 +17657,7 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B216" t="s">
         <v>75</v>
@@ -17677,7 +17671,7 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B217" t="s">
         <v>77</v>
@@ -17691,7 +17685,7 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B218" t="s">
         <v>79</v>
@@ -17705,7 +17699,7 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B219" t="s">
         <v>81</v>
@@ -17719,7 +17713,7 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B220" t="s">
         <v>81</v>
@@ -17733,7 +17727,7 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B221" t="s">
         <v>81</v>
@@ -17747,7 +17741,7 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B222" t="s">
         <v>81</v>
@@ -17761,7 +17755,7 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B223" t="s">
         <v>86</v>
@@ -17775,7 +17769,7 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B224" t="s">
         <v>88</v>
@@ -17789,7 +17783,7 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B225" t="s">
         <v>89</v>
@@ -17803,7 +17797,7 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B226" t="s">
         <v>91</v>
@@ -17817,7 +17811,7 @@
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B227" t="s">
         <v>93</v>
@@ -17831,7 +17825,7 @@
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B228" t="s">
         <v>95</v>
@@ -17845,7 +17839,7 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B229" t="s">
         <v>99</v>
@@ -17859,7 +17853,7 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B230" t="s">
         <v>102</v>
@@ -17873,7 +17867,7 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B231" t="s">
         <v>106</v>
@@ -17887,7 +17881,7 @@
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B232" t="s">
         <v>108</v>
@@ -17901,7 +17895,7 @@
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B233" t="s">
         <v>110</v>
@@ -17915,7 +17909,7 @@
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B234" t="s">
         <v>113</v>
@@ -17929,7 +17923,7 @@
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B235" t="s">
         <v>708</v>
@@ -17943,7 +17937,7 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B236" t="s">
         <v>114</v>
@@ -17957,7 +17951,7 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B237" t="s">
         <v>116</v>
@@ -17971,7 +17965,7 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B238" t="s">
         <v>118</v>
@@ -17985,7 +17979,7 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B239" t="s">
         <v>120</v>
@@ -17999,7 +17993,7 @@
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B240" t="s">
         <v>122</v>
@@ -18013,7 +18007,7 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B241" t="s">
         <v>709</v>
@@ -18027,7 +18021,7 @@
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B242" t="s">
         <v>123</v>
@@ -18041,7 +18035,7 @@
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B243" t="s">
         <v>126</v>
@@ -18055,7 +18049,7 @@
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B244" t="s">
         <v>128</v>
@@ -18069,7 +18063,7 @@
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B245" t="s">
         <v>132</v>
@@ -18083,7 +18077,7 @@
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B246" t="s">
         <v>134</v>
@@ -18097,7 +18091,7 @@
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B247" t="s">
         <v>135</v>
@@ -18111,7 +18105,7 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B248" t="s">
         <v>139</v>
@@ -18125,7 +18119,7 @@
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B249" t="s">
         <v>139</v>
@@ -18139,7 +18133,7 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B250" t="s">
         <v>142</v>
@@ -18153,7 +18147,7 @@
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B251" t="s">
         <v>145</v>
@@ -18167,7 +18161,7 @@
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B252" t="s">
         <v>147</v>
@@ -18181,7 +18175,7 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B253" t="s">
         <v>150</v>
@@ -18195,7 +18189,7 @@
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B254" t="s">
         <v>154</v>
@@ -18209,7 +18203,7 @@
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B255" t="s">
         <v>156</v>
@@ -18223,7 +18217,7 @@
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B256" t="s">
         <v>159</v>
@@ -18237,7 +18231,7 @@
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B257" t="s">
         <v>159</v>
@@ -18251,7 +18245,7 @@
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B258" t="s">
         <v>162</v>
@@ -18265,7 +18259,7 @@
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B259" t="s">
         <v>165</v>
@@ -18279,7 +18273,7 @@
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B260" t="s">
         <v>171</v>
@@ -18293,7 +18287,7 @@
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B261" t="s">
         <v>173</v>
@@ -18307,7 +18301,7 @@
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B262" t="s">
         <v>173</v>
@@ -18321,7 +18315,7 @@
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B263" t="s">
         <v>178</v>
@@ -18335,7 +18329,7 @@
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B264" t="s">
         <v>180</v>
@@ -18349,7 +18343,7 @@
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B265" t="s">
         <v>182</v>
@@ -18363,7 +18357,7 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B266" t="s">
         <v>185</v>
@@ -18377,7 +18371,7 @@
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B267" t="s">
         <v>187</v>
@@ -18391,7 +18385,7 @@
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B268" t="s">
         <v>189</v>
@@ -18405,7 +18399,7 @@
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B269" t="s">
         <v>191</v>
@@ -18419,7 +18413,7 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B270" t="s">
         <v>192</v>
@@ -18433,7 +18427,7 @@
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B271" t="s">
         <v>196</v>
@@ -18447,7 +18441,7 @@
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B272" t="s">
         <v>198</v>
@@ -18461,7 +18455,7 @@
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B273" t="s">
         <v>201</v>
@@ -18475,7 +18469,7 @@
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B274" t="s">
         <v>202</v>
@@ -18484,12 +18478,12 @@
         <v>1</v>
       </c>
       <c r="D274" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B275" t="s">
         <v>203</v>
@@ -18503,7 +18497,7 @@
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B276" t="s">
         <v>203</v>
@@ -18517,7 +18511,7 @@
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B277" t="s">
         <v>206</v>
@@ -18531,7 +18525,7 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B278" t="s">
         <v>207</v>
@@ -18545,7 +18539,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B279" t="s">
         <v>209</v>
@@ -18559,7 +18553,7 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B280" t="s">
         <v>211</v>
@@ -18573,7 +18567,7 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B281" t="s">
         <v>212</v>
@@ -18587,7 +18581,7 @@
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B282" t="s">
         <v>213</v>
@@ -18601,7 +18595,7 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B283" t="s">
         <v>215</v>
@@ -18615,7 +18609,7 @@
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B284" t="s">
         <v>218</v>
@@ -18629,7 +18623,7 @@
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B285" t="s">
         <v>224</v>
@@ -18643,7 +18637,7 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B286" t="s">
         <v>226</v>
@@ -18657,7 +18651,7 @@
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B287" t="s">
         <v>234</v>
@@ -18671,7 +18665,7 @@
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B288" t="s">
         <v>238</v>
@@ -18685,7 +18679,7 @@
     </row>
     <row r="289" spans="1:4">
       <c r="A289" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B289" t="s">
         <v>240</v>
@@ -18699,7 +18693,7 @@
     </row>
     <row r="290" spans="1:4">
       <c r="A290" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B290" t="s">
         <v>242</v>
@@ -18713,7 +18707,7 @@
     </row>
     <row r="291" spans="1:4">
       <c r="A291" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B291" t="s">
         <v>244</v>
@@ -18727,7 +18721,7 @@
     </row>
     <row r="292" spans="1:4">
       <c r="A292" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B292" t="s">
         <v>244</v>
@@ -18741,7 +18735,7 @@
     </row>
     <row r="293" spans="1:4">
       <c r="A293" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B293" t="s">
         <v>246</v>
@@ -18755,7 +18749,7 @@
     </row>
     <row r="294" spans="1:4">
       <c r="A294" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B294" t="s">
         <v>248</v>
@@ -18769,7 +18763,7 @@
     </row>
     <row r="295" spans="1:4">
       <c r="A295" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B295" t="s">
         <v>249</v>
@@ -18783,7 +18777,7 @@
     </row>
     <row r="296" spans="1:4">
       <c r="A296" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B296" t="s">
         <v>250</v>
@@ -18797,7 +18791,7 @@
     </row>
     <row r="297" spans="1:4">
       <c r="A297" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B297" t="s">
         <v>252</v>
@@ -18811,7 +18805,7 @@
     </row>
     <row r="298" spans="1:4">
       <c r="A298" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B298" t="s">
         <v>255</v>
@@ -18825,7 +18819,7 @@
     </row>
     <row r="299" spans="1:4">
       <c r="A299" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B299" t="s">
         <v>258</v>
@@ -18839,7 +18833,7 @@
     </row>
     <row r="300" spans="1:4">
       <c r="A300" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B300" t="s">
         <v>258</v>
@@ -18848,12 +18842,12 @@
         <v>1</v>
       </c>
       <c r="D300" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="301" spans="1:4">
       <c r="A301" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B301" t="s">
         <v>261</v>
@@ -18867,7 +18861,7 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B302" t="s">
         <v>711</v>
@@ -18881,7 +18875,7 @@
     </row>
     <row r="303" spans="1:4">
       <c r="A303" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B303" t="s">
         <v>264</v>
@@ -18895,7 +18889,7 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B304" t="s">
         <v>267</v>
@@ -18909,7 +18903,7 @@
     </row>
     <row r="305" spans="1:4">
       <c r="A305" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B305" t="s">
         <v>268</v>
@@ -18923,7 +18917,7 @@
     </row>
     <row r="306" spans="1:4">
       <c r="A306" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B306" t="s">
         <v>270</v>
@@ -18937,7 +18931,7 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B307" t="s">
         <v>272</v>
@@ -18951,7 +18945,7 @@
     </row>
     <row r="308" spans="1:4">
       <c r="A308" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B308" t="s">
         <v>275</v>
@@ -18965,7 +18959,7 @@
     </row>
     <row r="309" spans="1:4">
       <c r="A309" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B309" t="s">
         <v>278</v>
@@ -18979,7 +18973,7 @@
     </row>
     <row r="310" spans="1:4">
       <c r="A310" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B310" t="s">
         <v>278</v>
@@ -18988,12 +18982,12 @@
         <v>1</v>
       </c>
       <c r="D310" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="311" spans="1:4">
       <c r="A311" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B311" t="s">
         <v>281</v>
@@ -19007,7 +19001,7 @@
     </row>
     <row r="312" spans="1:4">
       <c r="A312" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B312" t="s">
         <v>283</v>
@@ -19021,7 +19015,7 @@
     </row>
     <row r="313" spans="1:4">
       <c r="A313" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B313" t="s">
         <v>284</v>
@@ -19035,7 +19029,7 @@
     </row>
     <row r="314" spans="1:4">
       <c r="A314" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B314" t="s">
         <v>286</v>
@@ -19049,7 +19043,7 @@
     </row>
     <row r="315" spans="1:4">
       <c r="A315" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B315" t="s">
         <v>288</v>
@@ -19063,7 +19057,7 @@
     </row>
     <row r="316" spans="1:4">
       <c r="A316" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B316" t="s">
         <v>290</v>
@@ -19077,7 +19071,7 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B317" t="s">
         <v>290</v>
@@ -19091,7 +19085,7 @@
     </row>
     <row r="318" spans="1:4">
       <c r="A318" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B318" t="s">
         <v>293</v>
@@ -19105,7 +19099,7 @@
     </row>
     <row r="319" spans="1:4">
       <c r="A319" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B319" t="s">
         <v>295</v>
@@ -19119,7 +19113,7 @@
     </row>
     <row r="320" spans="1:4">
       <c r="A320" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B320" t="s">
         <v>297</v>
@@ -19133,7 +19127,7 @@
     </row>
     <row r="321" spans="1:4">
       <c r="A321" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B321" t="s">
         <v>298</v>
@@ -19147,7 +19141,7 @@
     </row>
     <row r="322" spans="1:4">
       <c r="A322" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B322" t="s">
         <v>300</v>
@@ -19161,7 +19155,7 @@
     </row>
     <row r="323" spans="1:4">
       <c r="A323" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B323" t="s">
         <v>303</v>
@@ -19175,7 +19169,7 @@
     </row>
     <row r="324" spans="1:4">
       <c r="A324" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B324" t="s">
         <v>309</v>
@@ -19189,7 +19183,7 @@
     </row>
     <row r="325" spans="1:4">
       <c r="A325" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B325" t="s">
         <v>310</v>
@@ -19203,7 +19197,7 @@
     </row>
     <row r="326" spans="1:4">
       <c r="A326" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B326" t="s">
         <v>312</v>
@@ -19217,7 +19211,7 @@
     </row>
     <row r="327" spans="1:4">
       <c r="A327" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B327" t="s">
         <v>312</v>
@@ -19231,7 +19225,7 @@
     </row>
     <row r="328" spans="1:4">
       <c r="A328" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B328" t="s">
         <v>314</v>
@@ -19245,7 +19239,7 @@
     </row>
     <row r="329" spans="1:4">
       <c r="A329" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B329" t="s">
         <v>316</v>
@@ -19259,7 +19253,7 @@
     </row>
     <row r="330" spans="1:4">
       <c r="A330" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B330" t="s">
         <v>317</v>
@@ -19273,7 +19267,7 @@
     </row>
     <row r="331" spans="1:4">
       <c r="A331" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B331" t="s">
         <v>318</v>
@@ -19287,7 +19281,7 @@
     </row>
     <row r="332" spans="1:4">
       <c r="A332" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B332" t="s">
         <v>320</v>
@@ -19301,7 +19295,7 @@
     </row>
     <row r="333" spans="1:4">
       <c r="A333" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B333" t="s">
         <v>323</v>
@@ -19315,7 +19309,7 @@
     </row>
     <row r="334" spans="1:4">
       <c r="A334" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B334" t="s">
         <v>324</v>
@@ -19329,7 +19323,7 @@
     </row>
     <row r="335" spans="1:4">
       <c r="A335" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B335" t="s">
         <v>326</v>
@@ -19343,7 +19337,7 @@
     </row>
     <row r="336" spans="1:4">
       <c r="A336" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B336" t="s">
         <v>328</v>
@@ -19357,7 +19351,7 @@
     </row>
     <row r="337" spans="1:4">
       <c r="A337" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B337" t="s">
         <v>330</v>
@@ -19371,7 +19365,7 @@
     </row>
     <row r="338" spans="1:4">
       <c r="A338" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B338" t="s">
         <v>331</v>
@@ -19385,7 +19379,7 @@
     </row>
     <row r="339" spans="1:4">
       <c r="A339" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B339" t="s">
         <v>333</v>
@@ -19399,7 +19393,7 @@
     </row>
     <row r="340" spans="1:4">
       <c r="A340" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B340" t="s">
         <v>335</v>
@@ -19413,7 +19407,7 @@
     </row>
     <row r="341" spans="1:4">
       <c r="A341" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B341" t="s">
         <v>336</v>
@@ -19427,7 +19421,7 @@
     </row>
     <row r="342" spans="1:4">
       <c r="A342" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B342" t="s">
         <v>339</v>
@@ -19441,7 +19435,7 @@
     </row>
     <row r="343" spans="1:4">
       <c r="A343" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B343" t="s">
         <v>340</v>
@@ -19455,7 +19449,7 @@
     </row>
     <row r="344" spans="1:4">
       <c r="A344" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B344" t="s">
         <v>341</v>
@@ -19469,7 +19463,7 @@
     </row>
     <row r="345" spans="1:4">
       <c r="A345" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B345" t="s">
         <v>342</v>
@@ -19483,7 +19477,7 @@
     </row>
     <row r="346" spans="1:4">
       <c r="A346" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B346" t="s">
         <v>349</v>
@@ -19497,7 +19491,7 @@
     </row>
     <row r="347" spans="1:4">
       <c r="A347" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B347" t="s">
         <v>351</v>
@@ -19511,7 +19505,7 @@
     </row>
     <row r="348" spans="1:4">
       <c r="A348" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B348" t="s">
         <v>353</v>
@@ -19525,7 +19519,7 @@
     </row>
     <row r="349" spans="1:4">
       <c r="A349" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B349" t="s">
         <v>355</v>
@@ -19539,7 +19533,7 @@
     </row>
     <row r="350" spans="1:4">
       <c r="A350" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B350" t="s">
         <v>356</v>
@@ -19553,7 +19547,7 @@
     </row>
     <row r="351" spans="1:4">
       <c r="A351" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B351" t="s">
         <v>357</v>
@@ -19567,7 +19561,7 @@
     </row>
     <row r="352" spans="1:4">
       <c r="A352" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B352" t="s">
         <v>358</v>
@@ -19581,7 +19575,7 @@
     </row>
     <row r="353" spans="1:4">
       <c r="A353" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B353" t="s">
         <v>359</v>
@@ -19595,7 +19589,7 @@
     </row>
     <row r="354" spans="1:4">
       <c r="A354" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B354" t="s">
         <v>361</v>
@@ -19609,7 +19603,7 @@
     </row>
     <row r="355" spans="1:4">
       <c r="A355" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B355" t="s">
         <v>363</v>
@@ -19623,7 +19617,7 @@
     </row>
     <row r="356" spans="1:4">
       <c r="A356" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B356" t="s">
         <v>365</v>
@@ -19637,7 +19631,7 @@
     </row>
     <row r="357" spans="1:4">
       <c r="A357" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B357" t="s">
         <v>371</v>
@@ -19651,7 +19645,7 @@
     </row>
     <row r="358" spans="1:4">
       <c r="A358" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B358" t="s">
         <v>373</v>
@@ -19665,7 +19659,7 @@
     </row>
     <row r="359" spans="1:4">
       <c r="A359" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B359" t="s">
         <v>373</v>
@@ -19679,7 +19673,7 @@
     </row>
     <row r="360" spans="1:4">
       <c r="A360" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B360" t="s">
         <v>375</v>
@@ -19693,7 +19687,7 @@
     </row>
     <row r="361" spans="1:4">
       <c r="A361" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B361" t="s">
         <v>377</v>
@@ -19707,7 +19701,7 @@
     </row>
     <row r="362" spans="1:4">
       <c r="A362" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B362" t="s">
         <v>380</v>
@@ -19721,7 +19715,7 @@
     </row>
     <row r="363" spans="1:4">
       <c r="A363" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B363" t="s">
         <v>382</v>
@@ -19735,7 +19729,7 @@
     </row>
     <row r="364" spans="1:4">
       <c r="A364" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B364" t="s">
         <v>383</v>
@@ -19749,7 +19743,7 @@
     </row>
     <row r="365" spans="1:4">
       <c r="A365" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B365" t="s">
         <v>384</v>
@@ -19763,7 +19757,7 @@
     </row>
     <row r="366" spans="1:4">
       <c r="A366" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B366" t="s">
         <v>386</v>
@@ -19777,7 +19771,7 @@
     </row>
     <row r="367" spans="1:4">
       <c r="A367" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B367" t="s">
         <v>388</v>
@@ -19791,7 +19785,7 @@
     </row>
     <row r="368" spans="1:4">
       <c r="A368" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B368" t="s">
         <v>389</v>
@@ -19805,7 +19799,7 @@
     </row>
     <row r="369" spans="1:4">
       <c r="A369" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B369" t="s">
         <v>390</v>
@@ -19819,7 +19813,7 @@
     </row>
     <row r="370" spans="1:4">
       <c r="A370" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B370" t="s">
         <v>391</v>
@@ -19833,7 +19827,7 @@
     </row>
     <row r="371" spans="1:4">
       <c r="A371" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B371" t="s">
         <v>395</v>
@@ -19847,7 +19841,7 @@
     </row>
     <row r="372" spans="1:4">
       <c r="A372" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B372" t="s">
         <v>399</v>
@@ -19861,7 +19855,7 @@
     </row>
     <row r="373" spans="1:4">
       <c r="A373" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B373" t="s">
         <v>401</v>
@@ -19875,7 +19869,7 @@
     </row>
     <row r="374" spans="1:4">
       <c r="A374" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B374" t="s">
         <v>403</v>
@@ -19889,7 +19883,7 @@
     </row>
     <row r="375" spans="1:4">
       <c r="A375" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B375" t="s">
         <v>405</v>
@@ -19903,7 +19897,7 @@
     </row>
     <row r="376" spans="1:4">
       <c r="A376" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B376" t="s">
         <v>406</v>
@@ -19917,7 +19911,7 @@
     </row>
     <row r="377" spans="1:4">
       <c r="A377" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B377" t="s">
         <v>407</v>
@@ -19931,7 +19925,7 @@
     </row>
     <row r="378" spans="1:4">
       <c r="A378" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B378" t="s">
         <v>408</v>
@@ -19945,7 +19939,7 @@
     </row>
     <row r="379" spans="1:4">
       <c r="A379" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B379" t="s">
         <v>410</v>
@@ -19959,7 +19953,7 @@
     </row>
     <row r="380" spans="1:4">
       <c r="A380" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B380" t="s">
         <v>415</v>
@@ -19973,7 +19967,7 @@
     </row>
     <row r="381" spans="1:4">
       <c r="A381" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B381" t="s">
         <v>416</v>
@@ -19987,7 +19981,7 @@
     </row>
     <row r="382" spans="1:4">
       <c r="A382" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B382" t="s">
         <v>417</v>
@@ -20001,7 +19995,7 @@
     </row>
     <row r="383" spans="1:4">
       <c r="A383" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B383" t="s">
         <v>420</v>
@@ -20015,7 +20009,7 @@
     </row>
     <row r="384" spans="1:4">
       <c r="A384" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B384" t="s">
         <v>421</v>
@@ -20029,7 +20023,7 @@
     </row>
     <row r="385" spans="1:4">
       <c r="A385" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B385" t="s">
         <v>422</v>
@@ -20043,7 +20037,7 @@
     </row>
     <row r="386" spans="1:4">
       <c r="A386" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B386" t="s">
         <v>423</v>
@@ -20057,7 +20051,7 @@
     </row>
     <row r="387" spans="1:4">
       <c r="A387" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B387" t="s">
         <v>424</v>
@@ -20071,7 +20065,7 @@
     </row>
     <row r="388" spans="1:4">
       <c r="A388" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B388" t="s">
         <v>428</v>
@@ -20085,7 +20079,7 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B389" t="s">
         <v>429</v>
@@ -20099,7 +20093,7 @@
     </row>
     <row r="390" spans="1:4">
       <c r="A390" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B390" t="s">
         <v>430</v>
@@ -20113,7 +20107,7 @@
     </row>
     <row r="391" spans="1:4">
       <c r="A391" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B391" t="s">
         <v>433</v>
@@ -20127,7 +20121,7 @@
     </row>
     <row r="392" spans="1:4">
       <c r="A392" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B392" t="s">
         <v>435</v>
@@ -20141,7 +20135,7 @@
     </row>
     <row r="393" spans="1:4">
       <c r="A393" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B393" t="s">
         <v>436</v>
@@ -20155,7 +20149,7 @@
     </row>
     <row r="394" spans="1:4">
       <c r="A394" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B394" t="s">
         <v>438</v>
@@ -20169,7 +20163,7 @@
     </row>
     <row r="395" spans="1:4">
       <c r="A395" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B395" t="s">
         <v>439</v>
@@ -20183,7 +20177,7 @@
     </row>
     <row r="396" spans="1:4">
       <c r="A396" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B396" t="s">
         <v>442</v>
@@ -20197,7 +20191,7 @@
     </row>
     <row r="397" spans="1:4">
       <c r="A397" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B397" t="s">
         <v>443</v>
@@ -20211,7 +20205,7 @@
     </row>
     <row r="398" spans="1:4">
       <c r="A398" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B398" t="s">
         <v>445</v>
@@ -20225,7 +20219,7 @@
     </row>
     <row r="399" spans="1:4">
       <c r="A399" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B399" t="s">
         <v>447</v>
@@ -20239,7 +20233,7 @@
     </row>
     <row r="400" spans="1:4">
       <c r="A400" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B400" t="s">
         <v>449</v>
@@ -20253,7 +20247,7 @@
     </row>
     <row r="401" spans="1:4">
       <c r="A401" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B401" t="s">
         <v>450</v>
@@ -20267,7 +20261,7 @@
     </row>
     <row r="402" spans="1:4">
       <c r="A402" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B402" t="s">
         <v>452</v>
@@ -20281,7 +20275,7 @@
     </row>
     <row r="403" spans="1:4">
       <c r="A403" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B403" t="s">
         <v>454</v>
@@ -20295,7 +20289,7 @@
     </row>
     <row r="404" spans="1:4">
       <c r="A404" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B404" t="s">
         <v>456</v>
@@ -20309,7 +20303,7 @@
     </row>
     <row r="405" spans="1:4">
       <c r="A405" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B405" t="s">
         <v>461</v>
@@ -20323,7 +20317,7 @@
     </row>
     <row r="406" spans="1:4">
       <c r="A406" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B406" t="s">
         <v>463</v>
@@ -20337,7 +20331,7 @@
     </row>
     <row r="407" spans="1:4">
       <c r="A407" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B407" t="s">
         <v>465</v>
@@ -20351,7 +20345,7 @@
     </row>
     <row r="408" spans="1:4">
       <c r="A408" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B408" t="s">
         <v>466</v>
@@ -20365,7 +20359,7 @@
     </row>
     <row r="409" spans="1:4">
       <c r="A409" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B409" t="s">
         <v>468</v>
@@ -20379,7 +20373,7 @@
     </row>
     <row r="410" spans="1:4">
       <c r="A410" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B410" t="s">
         <v>470</v>
@@ -20393,7 +20387,7 @@
     </row>
     <row r="411" spans="1:4">
       <c r="A411" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B411" t="s">
         <v>473</v>
@@ -20407,7 +20401,7 @@
     </row>
     <row r="412" spans="1:4">
       <c r="A412" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B412" t="s">
         <v>481</v>
@@ -20421,7 +20415,7 @@
     </row>
     <row r="413" spans="1:4">
       <c r="A413" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B413" t="s">
         <v>485</v>
@@ -20435,7 +20429,7 @@
     </row>
     <row r="414" spans="1:4">
       <c r="A414" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B414" t="s">
         <v>486</v>
@@ -20449,7 +20443,7 @@
     </row>
     <row r="415" spans="1:4">
       <c r="A415" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B415" t="s">
         <v>489</v>
@@ -20463,7 +20457,7 @@
     </row>
     <row r="416" spans="1:4">
       <c r="A416" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B416" t="s">
         <v>491</v>
@@ -20477,7 +20471,7 @@
     </row>
     <row r="417" spans="1:4">
       <c r="A417" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B417" t="s">
         <v>493</v>
@@ -20491,7 +20485,7 @@
     </row>
     <row r="418" spans="1:4">
       <c r="A418" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B418" t="s">
         <v>495</v>
@@ -20505,7 +20499,7 @@
     </row>
     <row r="419" spans="1:4">
       <c r="A419" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B419" t="s">
         <v>497</v>
@@ -20519,7 +20513,7 @@
     </row>
     <row r="420" spans="1:4">
       <c r="A420" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B420" t="s">
         <v>498</v>
@@ -20533,7 +20527,7 @@
     </row>
     <row r="421" spans="1:4">
       <c r="A421" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B421" t="s">
         <v>499</v>
@@ -20547,7 +20541,7 @@
     </row>
     <row r="422" spans="1:4">
       <c r="A422" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B422" t="s">
         <v>500</v>
@@ -20561,7 +20555,7 @@
     </row>
     <row r="423" spans="1:4">
       <c r="A423" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B423" t="s">
         <v>504</v>
@@ -20575,7 +20569,7 @@
     </row>
     <row r="424" spans="1:4">
       <c r="A424" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B424" t="s">
         <v>504</v>
@@ -20589,7 +20583,7 @@
     </row>
     <row r="425" spans="1:4">
       <c r="A425" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B425" t="s">
         <v>507</v>
@@ -20603,7 +20597,7 @@
     </row>
     <row r="426" spans="1:4">
       <c r="A426" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B426" t="s">
         <v>508</v>
@@ -20617,7 +20611,7 @@
     </row>
     <row r="427" spans="1:4">
       <c r="A427" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B427" t="s">
         <v>509</v>
@@ -20631,7 +20625,7 @@
     </row>
     <row r="428" spans="1:4">
       <c r="A428" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B428" t="s">
         <v>510</v>
@@ -20645,7 +20639,7 @@
     </row>
     <row r="429" spans="1:4">
       <c r="A429" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B429" t="s">
         <v>511</v>
@@ -20659,7 +20653,7 @@
     </row>
     <row r="430" spans="1:4">
       <c r="A430" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B430" t="s">
         <v>511</v>
@@ -20673,7 +20667,7 @@
     </row>
     <row r="431" spans="1:4">
       <c r="A431" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B431" t="s">
         <v>512</v>
@@ -20687,7 +20681,7 @@
     </row>
     <row r="432" spans="1:4">
       <c r="A432" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B432" t="s">
         <v>700</v>
@@ -20701,7 +20695,7 @@
     </row>
     <row r="433" spans="1:4">
       <c r="A433" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B433" t="s">
         <v>514</v>
@@ -20715,7 +20709,7 @@
     </row>
     <row r="434" spans="1:4">
       <c r="A434" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B434" t="s">
         <v>516</v>
@@ -20729,7 +20723,7 @@
     </row>
     <row r="435" spans="1:4">
       <c r="A435" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B435" t="s">
         <v>517</v>
@@ -20743,7 +20737,7 @@
     </row>
     <row r="436" spans="1:4">
       <c r="A436" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B436" t="s">
         <v>519</v>
@@ -20757,7 +20751,7 @@
     </row>
     <row r="437" spans="1:4">
       <c r="A437" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B437" t="s">
         <v>523</v>
@@ -20771,7 +20765,7 @@
     </row>
     <row r="438" spans="1:4">
       <c r="A438" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B438" t="s">
         <v>525</v>
@@ -20785,7 +20779,7 @@
     </row>
     <row r="439" spans="1:4">
       <c r="A439" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B439" t="s">
         <v>527</v>
@@ -20799,7 +20793,7 @@
     </row>
     <row r="440" spans="1:4">
       <c r="A440" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B440" t="s">
         <v>529</v>
@@ -20813,7 +20807,7 @@
     </row>
     <row r="441" spans="1:4">
       <c r="A441" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B441" t="s">
         <v>530</v>
@@ -20827,7 +20821,7 @@
     </row>
     <row r="442" spans="1:4">
       <c r="A442" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B442" t="s">
         <v>531</v>
@@ -20841,7 +20835,7 @@
     </row>
     <row r="443" spans="1:4">
       <c r="A443" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B443" t="s">
         <v>533</v>
@@ -20855,7 +20849,7 @@
     </row>
     <row r="444" spans="1:4">
       <c r="A444" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B444" t="s">
         <v>533</v>
@@ -20869,7 +20863,7 @@
     </row>
     <row r="445" spans="1:4">
       <c r="A445" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B445" t="s">
         <v>537</v>
@@ -20883,7 +20877,7 @@
     </row>
     <row r="446" spans="1:4">
       <c r="A446" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B446" t="s">
         <v>537</v>
@@ -20897,7 +20891,7 @@
     </row>
     <row r="447" spans="1:4">
       <c r="A447" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B447" t="s">
         <v>539</v>
@@ -20911,7 +20905,7 @@
     </row>
     <row r="448" spans="1:4">
       <c r="A448" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B448" t="s">
         <v>539</v>
@@ -20925,7 +20919,7 @@
     </row>
     <row r="449" spans="1:4">
       <c r="A449" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B449" t="s">
         <v>542</v>
@@ -20939,7 +20933,7 @@
     </row>
     <row r="450" spans="1:4">
       <c r="A450" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B450" t="s">
         <v>543</v>
@@ -20953,7 +20947,7 @@
     </row>
     <row r="451" spans="1:4">
       <c r="A451" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B451" t="s">
         <v>545</v>
@@ -20967,7 +20961,7 @@
     </row>
     <row r="452" spans="1:4">
       <c r="A452" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B452" t="s">
         <v>546</v>
@@ -20981,7 +20975,7 @@
     </row>
     <row r="453" spans="1:4">
       <c r="A453" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B453" t="s">
         <v>548</v>
@@ -20995,7 +20989,7 @@
     </row>
     <row r="454" spans="1:4">
       <c r="A454" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B454" t="s">
         <v>549</v>
@@ -21009,7 +21003,7 @@
     </row>
     <row r="455" spans="1:4">
       <c r="A455" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B455" t="s">
         <v>551</v>
@@ -21023,7 +21017,7 @@
     </row>
     <row r="456" spans="1:4">
       <c r="A456" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B456" t="s">
         <v>552</v>
@@ -21037,7 +21031,7 @@
     </row>
     <row r="457" spans="1:4">
       <c r="A457" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B457" t="s">
         <v>553</v>
@@ -21051,7 +21045,7 @@
     </row>
     <row r="458" spans="1:4">
       <c r="A458" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B458" t="s">
         <v>555</v>
@@ -21065,7 +21059,7 @@
     </row>
     <row r="459" spans="1:4">
       <c r="A459" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B459" t="s">
         <v>557</v>
@@ -21079,7 +21073,7 @@
     </row>
     <row r="460" spans="1:4">
       <c r="A460" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B460" t="s">
         <v>559</v>
@@ -21093,7 +21087,7 @@
     </row>
     <row r="461" spans="1:4">
       <c r="A461" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B461" t="s">
         <v>559</v>
@@ -21107,7 +21101,7 @@
     </row>
     <row r="462" spans="1:4">
       <c r="A462" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B462" t="s">
         <v>561</v>
@@ -21121,7 +21115,7 @@
     </row>
     <row r="463" spans="1:4">
       <c r="A463" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B463" t="s">
         <v>562</v>
@@ -21135,7 +21129,7 @@
     </row>
     <row r="464" spans="1:4">
       <c r="A464" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B464" t="s">
         <v>702</v>
@@ -21149,7 +21143,7 @@
     </row>
     <row r="465" spans="1:4">
       <c r="A465" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B465" t="s">
         <v>563</v>
@@ -21163,7 +21157,7 @@
     </row>
     <row r="466" spans="1:4">
       <c r="A466" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B466" t="s">
         <v>563</v>
@@ -21177,7 +21171,7 @@
     </row>
     <row r="467" spans="1:4">
       <c r="A467" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B467" t="s">
         <v>566</v>
@@ -21191,7 +21185,7 @@
     </row>
     <row r="468" spans="1:4">
       <c r="A468" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B468" t="s">
         <v>568</v>
@@ -21205,7 +21199,7 @@
     </row>
     <row r="469" spans="1:4">
       <c r="A469" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B469" t="s">
         <v>570</v>
@@ -21219,7 +21213,7 @@
     </row>
     <row r="470" spans="1:4">
       <c r="A470" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B470" t="s">
         <v>571</v>
@@ -21233,7 +21227,7 @@
     </row>
     <row r="471" spans="1:4">
       <c r="A471" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B471" t="s">
         <v>573</v>
@@ -21247,7 +21241,7 @@
     </row>
     <row r="472" spans="1:4">
       <c r="A472" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B472" t="s">
         <v>578</v>
@@ -21261,7 +21255,7 @@
     </row>
     <row r="473" spans="1:4">
       <c r="A473" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B473" t="s">
         <v>582</v>
@@ -21275,7 +21269,7 @@
     </row>
     <row r="474" spans="1:4">
       <c r="A474" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B474" t="s">
         <v>583</v>
@@ -21289,7 +21283,7 @@
     </row>
     <row r="475" spans="1:4">
       <c r="A475" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B475" t="s">
         <v>584</v>
@@ -21303,7 +21297,7 @@
     </row>
     <row r="476" spans="1:4">
       <c r="A476" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B476" t="s">
         <v>587</v>
@@ -21317,7 +21311,7 @@
     </row>
     <row r="477" spans="1:4">
       <c r="A477" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B477" t="s">
         <v>589</v>
@@ -21331,7 +21325,7 @@
     </row>
     <row r="478" spans="1:4">
       <c r="A478" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B478" t="s">
         <v>590</v>
@@ -21345,7 +21339,7 @@
     </row>
     <row r="479" spans="1:4">
       <c r="A479" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B479" t="s">
         <v>591</v>
@@ -21359,7 +21353,7 @@
     </row>
     <row r="480" spans="1:4">
       <c r="A480" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B480" t="s">
         <v>595</v>
@@ -21373,7 +21367,7 @@
     </row>
     <row r="481" spans="1:4">
       <c r="A481" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B481" t="s">
         <v>596</v>
@@ -21387,7 +21381,7 @@
     </row>
     <row r="482" spans="1:4">
       <c r="A482" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B482" t="s">
         <v>598</v>
@@ -21401,7 +21395,7 @@
     </row>
     <row r="483" spans="1:4">
       <c r="A483" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B483" t="s">
         <v>601</v>
@@ -21415,7 +21409,7 @@
     </row>
     <row r="484" spans="1:4">
       <c r="A484" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B484" t="s">
         <v>603</v>
@@ -21429,7 +21423,7 @@
     </row>
     <row r="485" spans="1:4">
       <c r="A485" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B485" t="s">
         <v>604</v>
@@ -21443,7 +21437,7 @@
     </row>
     <row r="486" spans="1:4">
       <c r="A486" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B486" t="s">
         <v>605</v>
@@ -21457,7 +21451,7 @@
     </row>
     <row r="487" spans="1:4">
       <c r="A487" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B487" t="s">
         <v>606</v>
@@ -21471,7 +21465,7 @@
     </row>
     <row r="488" spans="1:4">
       <c r="A488" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B488" t="s">
         <v>609</v>
@@ -21485,7 +21479,7 @@
     </row>
     <row r="489" spans="1:4">
       <c r="A489" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B489" t="s">
         <v>611</v>
@@ -21499,7 +21493,7 @@
     </row>
     <row r="490" spans="1:4">
       <c r="A490" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B490" t="s">
         <v>612</v>
@@ -21513,7 +21507,7 @@
     </row>
     <row r="491" spans="1:4">
       <c r="A491" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B491" t="s">
         <v>613</v>
@@ -21527,7 +21521,7 @@
     </row>
     <row r="492" spans="1:4">
       <c r="A492" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B492" t="s">
         <v>616</v>
@@ -21541,7 +21535,7 @@
     </row>
     <row r="493" spans="1:4">
       <c r="A493" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B493" t="s">
         <v>622</v>
@@ -21555,7 +21549,7 @@
     </row>
     <row r="494" spans="1:4">
       <c r="A494" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B494" t="s">
         <v>624</v>
@@ -21569,7 +21563,7 @@
     </row>
     <row r="495" spans="1:4">
       <c r="A495" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B495" t="s">
         <v>628</v>
@@ -21583,7 +21577,7 @@
     </row>
     <row r="496" spans="1:4">
       <c r="A496" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B496" t="s">
         <v>632</v>
@@ -21597,7 +21591,7 @@
     </row>
     <row r="497" spans="1:4">
       <c r="A497" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B497" t="s">
         <v>634</v>
@@ -21611,7 +21605,7 @@
     </row>
     <row r="498" spans="1:4">
       <c r="A498" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B498" t="s">
         <v>637</v>
@@ -21625,7 +21619,7 @@
     </row>
     <row r="499" spans="1:4">
       <c r="A499" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B499" t="s">
         <v>639</v>
@@ -21639,7 +21633,7 @@
     </row>
     <row r="500" spans="1:4">
       <c r="A500" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B500" t="s">
         <v>639</v>
@@ -21653,7 +21647,7 @@
     </row>
     <row r="501" spans="1:4">
       <c r="A501" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B501" t="s">
         <v>639</v>
@@ -21667,7 +21661,7 @@
     </row>
     <row r="502" spans="1:4">
       <c r="A502" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B502" t="s">
         <v>642</v>
@@ -21681,7 +21675,7 @@
     </row>
     <row r="503" spans="1:4">
       <c r="A503" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B503" t="s">
         <v>645</v>
@@ -21695,7 +21689,7 @@
     </row>
     <row r="504" spans="1:4">
       <c r="A504" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B504" t="s">
         <v>646</v>
@@ -21709,7 +21703,7 @@
     </row>
     <row r="505" spans="1:4">
       <c r="A505" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B505" t="s">
         <v>647</v>
@@ -21723,7 +21717,7 @@
     </row>
     <row r="506" spans="1:4">
       <c r="A506" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B506" t="s">
         <v>650</v>
@@ -21737,7 +21731,7 @@
     </row>
     <row r="507" spans="1:4">
       <c r="A507" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B507" t="s">
         <v>652</v>
@@ -21751,7 +21745,7 @@
     </row>
     <row r="508" spans="1:4">
       <c r="A508" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B508" t="s">
         <v>653</v>
@@ -21765,7 +21759,7 @@
     </row>
     <row r="509" spans="1:4">
       <c r="A509" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B509" t="s">
         <v>655</v>
@@ -21779,7 +21773,7 @@
     </row>
     <row r="510" spans="1:4">
       <c r="A510" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B510" t="s">
         <v>656</v>
@@ -21793,7 +21787,7 @@
     </row>
     <row r="511" spans="1:4">
       <c r="A511" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B511" t="s">
         <v>704</v>
@@ -21807,7 +21801,7 @@
     </row>
     <row r="512" spans="1:4">
       <c r="A512" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B512" t="s">
         <v>658</v>
@@ -21821,7 +21815,7 @@
     </row>
     <row r="513" spans="1:4">
       <c r="A513" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B513" t="s">
         <v>659</v>
@@ -21835,7 +21829,7 @@
     </row>
     <row r="514" spans="1:4">
       <c r="A514" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B514" t="s">
         <v>660</v>
@@ -21849,7 +21843,7 @@
     </row>
     <row r="515" spans="1:4">
       <c r="A515" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B515" t="s">
         <v>661</v>
@@ -21863,7 +21857,7 @@
     </row>
     <row r="516" spans="1:4">
       <c r="A516" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B516" t="s">
         <v>662</v>
@@ -21877,7 +21871,7 @@
     </row>
     <row r="517" spans="1:4">
       <c r="A517" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B517" t="s">
         <v>663</v>
@@ -21891,7 +21885,7 @@
     </row>
     <row r="518" spans="1:4">
       <c r="A518" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B518" t="s">
         <v>666</v>
@@ -21905,7 +21899,7 @@
     </row>
     <row r="519" spans="1:4">
       <c r="A519" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B519" t="s">
         <v>668</v>
@@ -21919,7 +21913,7 @@
     </row>
     <row r="520" spans="1:4">
       <c r="A520" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B520" t="s">
         <v>669</v>
@@ -21933,7 +21927,7 @@
     </row>
     <row r="521" spans="1:4">
       <c r="A521" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B521" t="s">
         <v>673</v>
@@ -21947,7 +21941,7 @@
     </row>
     <row r="522" spans="1:4">
       <c r="A522" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B522" t="s">
         <v>675</v>
@@ -21961,7 +21955,7 @@
     </row>
     <row r="523" spans="1:4">
       <c r="A523" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B523" t="s">
         <v>680</v>
@@ -21975,7 +21969,7 @@
     </row>
     <row r="524" spans="1:4">
       <c r="A524" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B524" t="s">
         <v>681</v>
@@ -21989,7 +21983,7 @@
     </row>
     <row r="525" spans="1:4">
       <c r="A525" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B525" t="s">
         <v>682</v>
@@ -22003,7 +21997,7 @@
     </row>
     <row r="526" spans="1:4">
       <c r="A526" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B526" t="s">
         <v>684</v>
@@ -22017,7 +22011,7 @@
     </row>
     <row r="527" spans="1:4">
       <c r="A527" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B527" t="s">
         <v>686</v>
@@ -22031,7 +22025,7 @@
     </row>
     <row r="528" spans="1:4">
       <c r="A528" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B528" t="s">
         <v>689</v>
@@ -22045,7 +22039,7 @@
     </row>
     <row r="529" spans="1:4">
       <c r="A529" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B529" t="s">
         <v>693</v>
@@ -22059,7 +22053,7 @@
     </row>
     <row r="530" spans="1:4">
       <c r="A530" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B530" t="s">
         <v>696</v>
@@ -22072,7 +22066,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:AA533">
+  <sortState ref="B2:Z533">
     <sortCondition ref="C1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>